<commit_message>
fix: ward code on line 2054
</commit_message>
<xml_diff>
--- a/DANH MỤC VÀ MÃ SỐ CÁC ĐƠN VỊ HÀNH CHÍNH CẤP TỈNH.xlsx
+++ b/DANH MỤC VÀ MÃ SỐ CÁC ĐƠN VỊ HÀNH CHÍNH CẤP TỈNH.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thienbd/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thienbd/Desktop/GitRepo/vietnam-province-directory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922EA4BF-BB73-9B44-976A-8C4E7AC05AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA8B8A1-0367-3343-8522-DBDA916ABF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6647" uniqueCount="3031">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6646" uniqueCount="3030">
   <si>
     <t>Cấp tỉnh</t>
   </si>
@@ -9136,9 +9136,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Mã cấp xã/ phường</t>
   </si>
 </sst>
@@ -9147,7 +9144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -9234,10 +9231,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9534,8 +9531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3322"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A2032" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2054" sqref="C2054"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9554,7 +9551,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3030</v>
+        <v>3029</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -38295,8 +38292,8 @@
       <c r="B2054" s="1" t="s">
         <v>2054</v>
       </c>
-      <c r="C2054" s="5" t="s">
-        <v>3029</v>
+      <c r="C2054" s="5">
+        <v>21673</v>
       </c>
       <c r="D2054" s="3" t="s">
         <v>1937</v>

</xml_diff>